<commit_message>
biomass adjustment, evaporation term
</commit_message>
<xml_diff>
--- a/Yxs_table.xlsx
+++ b/Yxs_table.xlsx
@@ -482,7 +482,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="B2" t="n">
         <v>0.2</v>
@@ -502,16 +502,14 @@
       <c r="G2" t="n">
         <v>0.079</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+      <c r="H2" t="n">
+        <v>-0.07563566285451317</v>
       </c>
       <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="B3" t="n">
         <v>2.1</v>
@@ -532,15 +530,15 @@
         <v>0.104</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.9663990059210001</v>
+        <v>-0.04038692750915865</v>
       </c>
       <c r="I3" t="n">
-        <v>-4.545454545454588</v>
+        <v>13.63636363636376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="B4" t="n">
         <v>2.3</v>
@@ -560,13 +558,11 @@
       <c r="G4" t="n">
         <v>0.334</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+      <c r="H4" t="n">
+        <v>-0.07830535807649208</v>
       </c>
       <c r="I4" t="n">
-        <v>-9.090909090908992</v>
+        <v>-10.90909090909079</v>
       </c>
     </row>
     <row r="5">
@@ -592,10 +588,10 @@
         <v>0.357</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.156347057318155</v>
+        <v>0.07749399946415342</v>
       </c>
       <c r="I5" t="n">
-        <v>-2.261208576998047</v>
+        <v>-0.7407407407407398</v>
       </c>
     </row>
     <row r="6">
@@ -621,10 +617,10 @@
         <v>0.148</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.06895150811272871</v>
+        <v>0.02744298723289798</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.362637362637365</v>
+        <v>1.362637362637365</v>
       </c>
     </row>
     <row r="7">
@@ -640,7 +636,7 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>-0.02957726793635326</v>
+        <v>0.004971703331912686</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -657,13 +653,13 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>-0.02071836674413413</v>
+        <v>0.003958081394145274</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.9</v>
+        <v>4.9</v>
       </c>
       <c r="B9" t="n">
         <v>7.3</v>
@@ -684,13 +680,13 @@
         <v>0.141</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.01356485573484922</v>
+        <v>-0.02732858725059259</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.84</v>
+        <v>5.34</v>
       </c>
       <c r="B10" t="n">
         <v>8.300000000000001</v>
@@ -711,15 +707,15 @@
         <v>0.1</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.2210064321861178</v>
+        <v>-0.009624417043498451</v>
       </c>
       <c r="I10" t="n">
-        <v>6.784922394678495</v>
+        <v>0.9756097560975602</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.05</v>
+        <v>5.5</v>
       </c>
       <c r="B11" t="n">
         <v>9.300000000000001</v>
@@ -739,9 +735,11 @@
       <c r="G11" t="n">
         <v>0.156</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>0.009937416469076144</v>
+      </c>
       <c r="I11" t="n">
-        <v>1.692015209125475</v>
+        <v>0.3041825095057037</v>
       </c>
     </row>
     <row r="12">
@@ -767,10 +765,10 @@
         <v>0.058</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0981128683122864</v>
+        <v>0.0962391949236181</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3255607701119693</v>
+        <v>-0.1204685710062451</v>
       </c>
     </row>
     <row r="13">
@@ -796,10 +794,10 @@
         <v>0.048</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1127859293864221</v>
+        <v>0.1108251278555828</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.1674570243034973</v>
+        <v>0.1674570243034973</v>
       </c>
     </row>
     <row r="14">
@@ -825,10 +823,10 @@
         <v>0.031</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.1184773058079596</v>
+        <v>0.1165009817314631</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0795311845960653</v>
+        <v>0.0795311845960653</v>
       </c>
     </row>
     <row r="15">
@@ -854,10 +852,10 @@
         <v>0.025</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.1245197390795211</v>
+        <v>0.1227010535482061</v>
       </c>
       <c r="I15" t="n">
-        <v>0.003870967741935516</v>
+        <v>-0.003870967741935516</v>
       </c>
     </row>
     <row r="16">
@@ -883,10 +881,10 @@
         <v>0.153</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.1306001152136351</v>
+        <v>0.128686327541306</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.1232153334637199</v>
+        <v>0.1232153334637199</v>
       </c>
     </row>
     <row r="17">
@@ -912,10 +910,10 @@
         <v>0.204</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.1311353163590431</v>
+        <v>0.129310802540286</v>
       </c>
       <c r="I17" t="n">
-        <v>0.043124101581217</v>
+        <v>-0.043124101581217</v>
       </c>
     </row>
     <row r="18">
@@ -941,10 +939,10 @@
         <v>0.06900000000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.1332655952698377</v>
+        <v>0.1314085491721864</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.07067137809187272</v>
+        <v>0.07067137809187272</v>
       </c>
     </row>
     <row r="19">
@@ -970,10 +968,10 @@
         <v>0.041</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.1245710462189058</v>
+        <v>0.1234197296651822</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3991945036721156</v>
+        <v>-0.3991945036721156</v>
       </c>
     </row>
     <row r="20">
@@ -999,10 +997,10 @@
         <v>0.122</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.1262422973912199</v>
+        <v>0.1251522166491153</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0950413223140497</v>
+        <v>-0.0950413223140497</v>
       </c>
     </row>
     <row r="21">
@@ -1018,7 +1016,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-0.125180317792743</v>
+        <v>0.1248164347236817</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>

</xml_diff>